<commit_message>
variant 21 6 - 25
</commit_message>
<xml_diff>
--- a/variant_21/Задание 18/18.xlsx
+++ b/variant_21/Задание 18/18.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Admin\Desktop\Варианты\10 вариант\Файлы\Задание 18\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8025"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,8 +19,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -42,8 +37,16 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -54,6 +57,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFEDEDED"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -69,10 +78,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -133,7 +143,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -168,7 +178,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -345,7 +355,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -353,15 +363,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>55</v>
       </c>
@@ -402,7 +412,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>68</v>
       </c>
@@ -443,7 +453,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>24</v>
       </c>
@@ -484,7 +494,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>31</v>
       </c>
@@ -525,7 +535,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>34</v>
       </c>
@@ -566,7 +576,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>63</v>
       </c>
@@ -607,7 +617,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>25</v>
       </c>
@@ -648,7 +658,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>81</v>
       </c>
@@ -689,7 +699,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>35</v>
       </c>
@@ -730,7 +740,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>26</v>
       </c>
@@ -771,7 +781,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45</v>
       </c>
@@ -812,7 +822,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>55</v>
       </c>
@@ -853,7 +863,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>81</v>
       </c>
@@ -894,7 +904,714 @@
         <v>31</v>
       </c>
     </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <f t="shared" ref="A15:A26" si="0">A1 + MAX(,A16)</f>
+        <v>623</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" ref="B15:E15" si="1">B1 + MAX(A15,B16)</f>
+        <v>775</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="1"/>
+        <v>804</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="1"/>
+        <v>951</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="1"/>
+        <v>1024</v>
+      </c>
+      <c r="F15" s="1">
+        <f>F1 + MAX(E15,F16)</f>
+        <v>1142</v>
+      </c>
+      <c r="G15" s="2">
+        <f>G1 +F15 + H15</f>
+        <v>2415</v>
+      </c>
+      <c r="H15" s="1">
+        <f>H1 + MAX(I15,H16)</f>
+        <v>1223</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" ref="I15:M15" si="2">I1 + MAX(J15,I16)</f>
+        <v>1109</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" si="2"/>
+        <v>918</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" si="2"/>
+        <v>829</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="2"/>
+        <v>766</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" si="2"/>
+        <v>637</v>
+      </c>
+      <c r="O15" s="3">
+        <f>MAX(G15:G27)</f>
+        <v>2415</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <f t="shared" si="0"/>
+        <v>568</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" ref="B16:B27" si="3">B2 + MAX(A16,B17)</f>
+        <v>754</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" ref="C16:C27" si="4">C2 + MAX(B16,C17)</f>
+        <v>789</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" ref="D16:D27" si="5">D2 + MAX(C16,D17)</f>
+        <v>880</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" ref="E16:F27" si="6">E2 + MAX(D16,E17)</f>
+        <v>1000</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="6"/>
+        <v>1127</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" ref="G16:G27" si="7">G2 +F16 + H16</f>
+        <v>2399</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" ref="H16:H27" si="8">H2 + MAX(I16,H17)</f>
+        <v>1192</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" ref="I16:I27" si="9">I2 + MAX(J16,I17)</f>
+        <v>1027</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" ref="J16:J27" si="10">J2 + MAX(K16,J17)</f>
+        <v>836</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" ref="K16:K27" si="11">K2 + MAX(L16,K17)</f>
+        <v>788</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" ref="L16:L27" si="12">L2 + MAX(M16,L17)</f>
+        <v>701</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" ref="M16:M27" si="13">M2 + MAX(N16,M17)</f>
+        <v>556</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" si="3"/>
+        <v>674</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="4"/>
+        <v>751</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="5"/>
+        <v>795</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="6"/>
+        <v>982</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" ref="F17:F27" si="14">F3 + MAX(E17,F18)</f>
+        <v>1077</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="7"/>
+        <v>2278</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="8"/>
+        <v>1101</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="9"/>
+        <v>988</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="10"/>
+        <v>726</v>
+      </c>
+      <c r="K17" s="1">
+        <f t="shared" si="11"/>
+        <v>673</v>
+      </c>
+      <c r="L17" s="1">
+        <f t="shared" si="12"/>
+        <v>662</v>
+      </c>
+      <c r="M17" s="1">
+        <f t="shared" si="13"/>
+        <v>493</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <f t="shared" si="0"/>
+        <v>476</v>
+      </c>
+      <c r="B18" s="1">
+        <f t="shared" si="3"/>
+        <v>632</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="4"/>
+        <v>685</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="5"/>
+        <v>783</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="6"/>
+        <v>904</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="14"/>
+        <v>1032</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="7"/>
+        <v>2087</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="8"/>
+        <v>1024</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="9"/>
+        <v>894</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="10"/>
+        <v>710</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="11"/>
+        <v>623</v>
+      </c>
+      <c r="L18" s="1">
+        <f t="shared" si="12"/>
+        <v>583</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" si="13"/>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <f t="shared" si="0"/>
+        <v>445</v>
+      </c>
+      <c r="B19" s="1">
+        <f t="shared" si="3"/>
+        <v>609</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="4"/>
+        <v>658</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="5"/>
+        <v>699</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="6"/>
+        <v>847</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="14"/>
+        <v>942</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="7"/>
+        <v>1947</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="8"/>
+        <v>964</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" si="9"/>
+        <v>875</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" si="10"/>
+        <v>680</v>
+      </c>
+      <c r="K19" s="1">
+        <f t="shared" si="11"/>
+        <v>567</v>
+      </c>
+      <c r="L19" s="1">
+        <f t="shared" si="12"/>
+        <v>549</v>
+      </c>
+      <c r="M19" s="1">
+        <f t="shared" si="13"/>
+        <v>416</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <f t="shared" si="0"/>
+        <v>411</v>
+      </c>
+      <c r="B20" s="1">
+        <f t="shared" si="3"/>
+        <v>593</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="4"/>
+        <v>621</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="5"/>
+        <v>670</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="6"/>
+        <v>779</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="14"/>
+        <v>849</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="7"/>
+        <v>1740</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="8"/>
+        <v>868</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" si="9"/>
+        <v>782</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" si="10"/>
+        <v>622</v>
+      </c>
+      <c r="K20" s="1">
+        <f t="shared" si="11"/>
+        <v>548</v>
+      </c>
+      <c r="L20" s="1">
+        <f t="shared" si="12"/>
+        <v>506</v>
+      </c>
+      <c r="M20" s="1">
+        <f t="shared" si="13"/>
+        <v>351</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <f t="shared" si="0"/>
+        <v>348</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" si="3"/>
+        <v>520</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="4"/>
+        <v>550</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="5"/>
+        <v>611</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="6"/>
+        <v>682</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="14"/>
+        <v>710</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="7"/>
+        <v>1568</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="8"/>
+        <v>828</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" si="9"/>
+        <v>738</v>
+      </c>
+      <c r="J21" s="1">
+        <f t="shared" si="10"/>
+        <v>573</v>
+      </c>
+      <c r="K21" s="1">
+        <f t="shared" si="11"/>
+        <v>514</v>
+      </c>
+      <c r="L21" s="1">
+        <f t="shared" si="12"/>
+        <v>480</v>
+      </c>
+      <c r="M21" s="1">
+        <f t="shared" si="13"/>
+        <v>301</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <f t="shared" si="0"/>
+        <v>323</v>
+      </c>
+      <c r="B22" s="1">
+        <f t="shared" si="3"/>
+        <v>480</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="4"/>
+        <v>530</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="5"/>
+        <v>587</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="6"/>
+        <v>657</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="14"/>
+        <v>673</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="7"/>
+        <v>1489</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="8"/>
+        <v>760</v>
+      </c>
+      <c r="I22" s="1">
+        <f t="shared" si="9"/>
+        <v>697</v>
+      </c>
+      <c r="J22" s="1">
+        <f t="shared" si="10"/>
+        <v>560</v>
+      </c>
+      <c r="K22" s="1">
+        <f t="shared" si="11"/>
+        <v>499</v>
+      </c>
+      <c r="L22" s="1">
+        <f t="shared" si="12"/>
+        <v>420</v>
+      </c>
+      <c r="M22" s="1">
+        <f t="shared" si="13"/>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <f t="shared" si="0"/>
+        <v>242</v>
+      </c>
+      <c r="B23" s="1">
+        <f t="shared" si="3"/>
+        <v>387</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" si="4"/>
+        <v>460</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="5"/>
+        <v>493</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="6"/>
+        <v>504</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="14"/>
+        <v>623</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="7"/>
+        <v>1408</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="8"/>
+        <v>690</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" si="9"/>
+        <v>639</v>
+      </c>
+      <c r="J23" s="1">
+        <f t="shared" si="10"/>
+        <v>513</v>
+      </c>
+      <c r="K23" s="1">
+        <f t="shared" si="11"/>
+        <v>414</v>
+      </c>
+      <c r="L23" s="1">
+        <f t="shared" si="12"/>
+        <v>396</v>
+      </c>
+      <c r="M23" s="1">
+        <f t="shared" si="13"/>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <f t="shared" si="0"/>
+        <v>207</v>
+      </c>
+      <c r="B24" s="1">
+        <f t="shared" si="3"/>
+        <v>331</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" si="4"/>
+        <v>394</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="5"/>
+        <v>404</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="6"/>
+        <v>490</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="14"/>
+        <v>544</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="7"/>
+        <v>1280</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="8"/>
+        <v>666</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" si="9"/>
+        <v>572</v>
+      </c>
+      <c r="J24" s="1">
+        <f t="shared" si="10"/>
+        <v>488</v>
+      </c>
+      <c r="K24" s="1">
+        <f t="shared" si="11"/>
+        <v>401</v>
+      </c>
+      <c r="L24" s="1">
+        <f t="shared" si="12"/>
+        <v>306</v>
+      </c>
+      <c r="M24" s="1">
+        <f t="shared" si="13"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <f t="shared" si="0"/>
+        <v>181</v>
+      </c>
+      <c r="B25" s="1">
+        <f t="shared" si="3"/>
+        <v>279</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" si="4"/>
+        <v>294</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="5"/>
+        <v>366</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="6"/>
+        <v>412</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="14"/>
+        <v>498</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="7"/>
+        <v>1086</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="8"/>
+        <v>509</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" si="9"/>
+        <v>419</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" si="10"/>
+        <v>308</v>
+      </c>
+      <c r="K25" s="1">
+        <f t="shared" si="11"/>
+        <v>284</v>
+      </c>
+      <c r="L25" s="1">
+        <f t="shared" si="12"/>
+        <v>244</v>
+      </c>
+      <c r="M25" s="1">
+        <f t="shared" si="13"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <f t="shared" si="0"/>
+        <v>136</v>
+      </c>
+      <c r="B26" s="1">
+        <f t="shared" si="3"/>
+        <v>204</v>
+      </c>
+      <c r="C26" s="1">
+        <f t="shared" si="4"/>
+        <v>243</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="5"/>
+        <v>315</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="6"/>
+        <v>384</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="14"/>
+        <v>440</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="7"/>
+        <v>952</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="8"/>
+        <v>454</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="9"/>
+        <v>362</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" si="10"/>
+        <v>264</v>
+      </c>
+      <c r="K26" s="1">
+        <f t="shared" si="11"/>
+        <v>230</v>
+      </c>
+      <c r="L26" s="1">
+        <f t="shared" si="12"/>
+        <v>181</v>
+      </c>
+      <c r="M26" s="1">
+        <f t="shared" si="13"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <f>A13 + MAX(,A28)</f>
+        <v>81</v>
+      </c>
+      <c r="B27" s="1">
+        <f t="shared" si="3"/>
+        <v>169</v>
+      </c>
+      <c r="C27" s="1">
+        <f t="shared" si="4"/>
+        <v>224</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="5"/>
+        <v>237</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="6"/>
+        <v>318</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="14"/>
+        <v>413</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="7"/>
+        <v>850</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="8"/>
+        <v>370</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" si="9"/>
+        <v>275</v>
+      </c>
+      <c r="J27" s="1">
+        <f t="shared" si="10"/>
+        <v>221</v>
+      </c>
+      <c r="K27" s="1">
+        <f t="shared" si="11"/>
+        <v>172</v>
+      </c>
+      <c r="L27" s="1">
+        <f t="shared" si="12"/>
+        <v>109</v>
+      </c>
+      <c r="M27" s="1">
+        <f t="shared" si="13"/>
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>